<commit_message>
Updated tokenizer and model
</commit_message>
<xml_diff>
--- a/top_words_unclassified_words.xlsx
+++ b/top_words_unclassified_words.xlsx
@@ -477,11 +477,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>35519</v>
+        <v>31135</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>lgl - fidelity bank statement 10.31.2024_49daaf8f-3e14-435d-9204-e4cbe09a522d2024-11-04t15-28-30.pdf</t>
+          <t>us census - lgl partners llc_6b30e4b0-507a-4067-8d74-093d1085972e2024-10-29t08-40-34.pdf</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -493,7 +493,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>18340</v>
+        <v>15788</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8092</v>
+        <v>7060</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -541,7 +541,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5424</v>
+        <v>4686</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -553,15 +553,15 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>msg</t>
+          <t>fos</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4316</v>
+        <v>3745</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>fft - elements advanced part 2 training recording - 11.06.msg</t>
+          <t>vague - richard vague 2011 trust - lgl fos agreement_4e7b95b6-82c6-4376-98ec-003b72b5d4232024-04-17t12-32-00.pdf</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -569,15 +569,15 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>fos</t>
+          <t>ira</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4104</v>
+        <v>3692</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>eh fos accounts 12.31.13 statement.pdf</t>
+          <t>2023us pamg105.002 k1p v1 92 nfs_fmtc fbo keith m bloomfield ira _6d94a27b-acdd-4119-8468-033bdc425aaf2024-09-06t15-49-50.pdf</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -585,15 +585,15 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ltd</t>
+          <t>msg</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3904</v>
+        <v>3463</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>custer - decatur investments ltd.pdf</t>
+          <t>fft - elements advanced part 2 training recording - 11.06.msg</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -601,15 +601,15 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ira</t>
+          <t>ltd</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3876</v>
+        <v>3402</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2023us pamg105.002 k1p v1 92 nfs_fmtc fbo keith m bloomfield ira _6d94a27b-acdd-4119-8468-033bdc425aaf2024-09-06t15-49-50.pdf</t>
+          <t>unity master fund ltd. - appointment of first directors 2017.03.16 -_103ff734-8064-4138-9a54-7089298f2b6a2024-10-11t11-55-24.pdf</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -621,7 +621,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3616</v>
+        <v>3354</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3056</v>
+        <v>3055</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -653,11 +653,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3007</v>
+        <v>2921</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>alternative investments - shortcut_647f4ab8-8773-41ce-80f7-19c60cba33222024-04-12t13-38-56.lnk</t>
+          <t>bbg (fpserverglobal share) (r) - shortcut.lnk</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -669,7 +669,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2872</v>
+        <v>2840</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2530</v>
+        <v>2281</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -701,7 +701,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2192</v>
+        <v>2047</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -760,15 +760,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>presentation</t>
+          <t>transactions</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1639</v>
+        <v>1303</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>fft ventures - internal presentation.6.27.2024.pdf</t>
+          <t>transactions reliant.png</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -776,15 +776,15 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>transactions</t>
+          <t>alternatives</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1512</v>
+        <v>1254</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>transactions reliant.png</t>
+          <t>reuter family alternatives - q1 2024.pdf</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -792,15 +792,15 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>alternatives</t>
+          <t>distribution</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1331</v>
+        <v>906</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>reuter family alternatives - q1 2024.pdf</t>
+          <t>distribution 28-august-2024_monika owens .pdf</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -808,15 +808,15 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>distribution</t>
+          <t>confirmation</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>958</v>
+        <v>692</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>distribution 28-august-2024_monika owens .pdf</t>
+          <t>08312024_dprstslp_dprstslp-ip_administrator confirmation statement__3a633e12-9dee-4055-9fc8-f40501c083992024-11-06t15-46-33.pdf</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -824,15 +824,15 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>confirmation</t>
+          <t>consolidated</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>838</v>
+        <v>629</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>08312024_dprstslp_dprstslp-ip_administrator confirmation statement__3a633e12-9dee-4055-9fc8-f40501c083992024-11-06t15-46-33.pdf</t>
+          <t>lee katie consolidated.pdf</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -840,15 +840,15 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>consolidated</t>
+          <t>reallocation</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>815</v>
+        <v>507</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>lee katie consolidated.pdf</t>
+          <t>reallocation</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -856,15 +856,15 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>reallocation</t>
+          <t>kleinschmidt</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>519</v>
+        <v>466</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>reallocation</t>
+          <t>idt 2020 trust_the kevin kleinschmidt 2020 trust - 2023 estimate k-1_1bf24cf1-b0d0-4237-a252-ab6ad953d89b2024-09-17t12-46-17.pdf</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -872,15 +872,15 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>kleinschmidt</t>
+          <t>qbbackuptemp</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>488</v>
+        <v>460</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>idt 2020 trust_the kevin kleinschmidt 2020 trust - 2023 estimate k-1_1bf24cf1-b0d0-4237-a252-ab6ad953d89b2024-09-17t12-46-17.pdf</t>
+          <t>qbbackuptemp tue, oct 07 2014 11 28 45 am</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -888,15 +888,15 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>qbbackuptemp</t>
+          <t>philadelphia</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>460</v>
+        <v>300</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>qbbackuptemp tue, oct 07 2014 11 28 45 am</t>
+          <t>fft philadelphia visitors guide.pdf</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -904,15 +904,15 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>philadelphia</t>
+          <t>descriptions</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>414</v>
+        <v>295</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>fft philadelphia visitors guide.pdf</t>
+          <t>lgl -  alternatives descriptions.docx</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -920,15 +920,15 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>instructions</t>
+          <t>ab_histogram</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>366</v>
+        <v>279</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>llr standing instructions.xlsx</t>
+          <t>ab_histogram.aspx.cs</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -936,15 +936,15 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>descriptions</t>
+          <t>contribution</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>325</v>
+        <v>267</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>lgl -  alternatives descriptions.docx</t>
+          <t>kleinschmidt contribution schwab 3.2024.pdf</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -952,15 +952,15 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>contribution</t>
+          <t>breckinridge</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>297</v>
+        <v>163</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>kleinschmidt contribution schwab 3.2024.pdf</t>
+          <t>breckinridge</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -968,15 +968,15 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ab_histogram</t>
+          <t>conservative</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>279</v>
+        <v>161</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ab_histogram.aspx.cs</t>
+          <t>fft - ab - invesco conservative income inst.pdf</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -984,15 +984,15 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>applications</t>
+          <t>quantitative</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>217</v>
+        <v>144</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>andreessen horowitz fund ix - ai applications lp</t>
+          <t>moab - quantitative statistics.xlsx</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -1051,7 +1051,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>26475</v>
+        <v>23693</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1063,15 +1063,15 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>cash</t>
+          <t>data</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9567</v>
+        <v>8697</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>lieberman cash.png</t>
+          <t>fft market data template.xlsx</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -1079,15 +1079,15 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>data</t>
+          <t>cash</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8807</v>
+        <v>8667</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>fft market data template.xlsx</t>
+          <t>lieberman cash.png</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -1099,7 +1099,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5337</v>
+        <v>4863</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1115,11 +1115,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4463</v>
+        <v>3940</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>copy of gemsstock attributions (master sheet) august 2024.xlsx</t>
+          <t>copy of bd recon accounts.xlsx</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -1131,7 +1131,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3294</v>
+        <v>3117</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1143,15 +1143,15 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>core</t>
+          <t>aspx</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2796</v>
+        <v>2621</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>core estimates.xlsx</t>
+          <t>home.aspx</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -1159,15 +1159,15 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>aspx</t>
+          <t>core</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2625</v>
+        <v>2578</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>home.aspx</t>
+          <t>core estimates.xlsx</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -1175,15 +1175,15 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>list</t>
+          <t>docs</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2375</v>
+        <v>2148</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3q24 newsletter mailing list.xlsx</t>
+          <t>adler general docs</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -1191,15 +1191,15 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>docs</t>
+          <t>list</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2184</v>
+        <v>1957</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>adler general docs</t>
+          <t>3q24 newsletter mailing list.xlsx</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -1207,15 +1207,15 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>june</t>
+          <t>citi</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2081</v>
+        <v>1949</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>team coverage june 2024.xlsx</t>
+          <t>citi private bank</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -1227,11 +1227,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2049</v>
+        <v>1747</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>bala 4 &amp; 5 - ytd, attribution.pdf</t>
+          <t>bala reimb - fwm 2023_1d76f7cf-dd96-41dc-a236-68246e92f9462023-11-07t09-27-55.xlsx</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -1239,15 +1239,15 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>citi</t>
+          <t>june</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1977</v>
+        <v>1580</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>citi private bank</t>
+          <t>team coverage june 2024.xlsx</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -1255,15 +1255,15 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>item</t>
+          <t>stmt</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1799</v>
+        <v>1474</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>item 12.14  - forbes license agreement_57ac1005-5fd3-4d10-b277-d3798cebf2812024-03-26t12-56-32.pdf</t>
+          <t>2023.4 amgcf stmt haupt jason &amp; paige_88126240-f418-48b3-9b82-e6658ab945692023-06-27t16-48-08.pdf</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -1271,15 +1271,15 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>wire</t>
+          <t>csfb</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1772</v>
+        <v>1423</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>jcm wire.png</t>
+          <t>may 2014 csfb analysis</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -1338,7 +1338,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8404</v>
+        <v>7865</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1354,7 +1354,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2996</v>
+        <v>2840</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1366,15 +1366,15 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>class</t>
+          <t>check</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2787</v>
+        <v>2633</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>october 2024 dgvp ii class c.pdf</t>
+          <t>remote check deposits.xlsx</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -1382,15 +1382,15 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>check</t>
+          <t>class</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2729</v>
+        <v>2589</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>remote check deposits.xlsx</t>
+          <t>october 2024 dgvp ii class c.pdf</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -1398,15 +1398,15 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>asset</t>
+          <t>funds</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2426</v>
+        <v>2055</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>open_protocol_one river asset management, llc_ordcsp_09302024.xlsx</t>
+          <t>hedge funds</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -1418,11 +1418,11 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2389</v>
+        <v>1973</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>note 10.23.24 final.pdf</t>
+          <t>infinity select ii subpack 2024-08 final.pdf</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -1430,15 +1430,15 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>funds</t>
+          <t>asset</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2286</v>
+        <v>1893</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>hedge funds</t>
+          <t>08-2024 canyon value realization fund, l_p_ (vrf) top 5 by asset class (final).pdf</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -1446,15 +1446,15 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>draft</t>
+          <t>adler</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1983</v>
+        <v>1685</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>criteria for selection - fft draft v2 bos_d1dde306-7535-43de-a0d8-15f34526ca312024-10-10t10-02-57.docx</t>
+          <t>adler jeff and rita.pdf</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -1462,15 +1462,15 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>adler</t>
+          <t>indiv</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1821</v>
+        <v>1451</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>adler jrappi ppli policy.pdf</t>
+          <t>nancy corkin indiv.csv</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1776</v>
+        <v>1303</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1498,11 +1498,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1523</v>
+        <v>1211</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>gmo adv part 2b - april 2024 final (2).pdf</t>
+          <t>gtf exposure snapshot - april 2021.xlsx</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -1510,15 +1510,15 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>indiv</t>
+          <t>value</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1491</v>
+        <v>1120</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>nancy corkin indiv.csv</t>
+          <t>08-2024 canyon value realization fund, l_p_ (vrf) top 5 by asset class (final).pdf</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -1526,15 +1526,15 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>prime</t>
+          <t>joint</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1321</v>
+        <v>1115</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>subdocs - prime storage fund ii cv llc ex.pdf</t>
+          <t>sam fido joint statement7312024.pdf</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -1542,15 +1542,15 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>trade</t>
+          <t>prime</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1261</v>
+        <v>1098</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>trade diagnostics_5639ca55-f66b-4c8a-89c2-e75a9959cd572024-08-26t20-54-23.xlsx</t>
+          <t>subdocs - prime storage fund ii cv llc ex.pdf</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -1558,15 +1558,15 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>joint</t>
+          <t>haron</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1226</v>
+        <v>1002</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>sam fido joint statement7312024.pdf</t>
+          <t>haron - review - q1 2024.pdf</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -1625,11 +1625,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6012</v>
+        <v>5030</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>optima global trading fund manager profiles 10_31_24.pptx</t>
+          <t>optima global trading fund overview (10-31-24).pptx</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -1641,11 +1641,11 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4677</v>
+        <v>4399</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>gemsstock attributions (master sheet) may14-sep24.xlsx</t>
+          <t>unity master fund ltd. - appointment of first directors 2017.03.16 -_103ff734-8064-4138-9a54-7089298f2b6a2024-10-11t11-55-24.pdf</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -1657,7 +1657,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4548</v>
+        <v>3654</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1673,7 +1673,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3200</v>
+        <v>2804</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1689,11 +1689,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2997</v>
+        <v>2550</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>optima healthcare &amp; biotech manager profiles september 24.pptx</t>
+          <t>optima healthcare and biotech fund overview september 24.pptx</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2855</v>
+        <v>2463</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1717,15 +1717,15 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>market</t>
+          <t>thumbs</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2277</v>
+        <v>2205</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>fft market data template.xlsx</t>
+          <t>thumbs.db</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -1733,15 +1733,15 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>thumbs</t>
+          <t>market</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2205</v>
+        <v>2175</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>thumbs.db</t>
+          <t>fft market data template.xlsx</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -1749,15 +1749,15 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>letter</t>
+          <t>trades</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2118</v>
+        <v>1931</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>soleus q3 2024 letter.pdf</t>
+          <t>trades 09.30.2024 to 10.04.2024.xlsx</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -1769,7 +1769,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2033</v>
+        <v>1828</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1785,7 +1785,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2021</v>
+        <v>1826</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1797,15 +1797,15 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>trades</t>
+          <t>forbes</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1947</v>
+        <v>1522</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>trades 09.30.2024 to 10.04.2024.xlsx</t>
+          <t>forbes robert &amp; lydia consolidated.pdf</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -1813,15 +1813,15 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>forbes</t>
+          <t>averyt</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1716</v>
+        <v>1392</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>forbes robert &amp; lydia consolidated.pdf</t>
+          <t>2024.09.30 gayle averyt 1991 crut_8a9c5358-675a-4a0e-b798-262b188db1762024-10-24t12-06-11.pdf</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -1829,15 +1829,15 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>select</t>
+          <t>series</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1541</v>
+        <v>1198</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>infinity select ii subpack 2024-08 final.pdf</t>
+          <t>12 31 23 afs review of canyon value realization fund lp - series a.docx</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -1845,15 +1845,15 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>report</t>
+          <t>select</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1520</v>
+        <v>1172</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>paradigm biocapital - october 2024 report.pdf</t>
+          <t>infinity select ii subpack 2024-08 final.pdf</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -1912,7 +1912,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3153</v>
+        <v>2855</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2822</v>
+        <v>2347</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1944,7 +1944,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1973</v>
+        <v>1910</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1956,15 +1956,15 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>manager</t>
+          <t>spcolor</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1838</v>
+        <v>1506</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>optima healthcare &amp; biotech manager profiles september 24.pptx</t>
+          <t>palette004.spcolor</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -1972,15 +1972,15 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>spcolor</t>
+          <t>richard</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1506</v>
+        <v>1380</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>palette004.spcolor</t>
+          <t>sager richard revocable trust.pdf</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -1988,15 +1988,15 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>richard</t>
+          <t>lenfest</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1488</v>
+        <v>1222</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>sager richard revocable trust.pdf</t>
+          <t>lenfest, brook.lnk</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -2004,15 +2004,15 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>lenfest</t>
+          <t>harvest</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1398</v>
+        <v>1032</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>lenfest, brook.lnk</t>
+          <t>12 31 23 afs review of harvest mlp income fund llc_a6ca6609-d183-4dfa-a8aa-1d6cba6d38bf2024-07-26t15-39-14.docx</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -2020,15 +2020,15 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>january</t>
+          <t>request</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1242</v>
+        <v>1030</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>atomiclabsii_atomic labs ii l.p. - lp privacy notice (final - january 2024).pdf</t>
+          <t>fft data request vfinal.pdf</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -2040,11 +2040,11 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1231</v>
+        <v>980</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>atomiclabsii_plum private investments llc_4q 23 cap statement .pdf</t>
+          <t>private credit iii, llc - 2023 federal k-1 (1)_48fdd12c-cfe6-4fd9-93b1-ce3fdb84f1672024-08-27t08-19-49.pdf</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -2052,15 +2052,15 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>october</t>
+          <t>trading</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1180</v>
+        <v>970</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>october 2024 dgvp ii class c.pdf</t>
+          <t>optima global trading fund overview (10-31-24).pptx</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -2068,15 +2068,15 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>request</t>
+          <t>january</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1159</v>
+        <v>961</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>fft data request vfinal.pdf</t>
+          <t>atomiclabsii_atomic labs ii l.p. - lp privacy notice (final - january 2024).pdf</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -2084,15 +2084,15 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>harvest</t>
+          <t>october</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1147</v>
+        <v>907</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>12 31 23 afs review of harvest mlp income fund llc_a6ca6609-d183-4dfa-a8aa-1d6cba6d38bf2024-07-26t15-39-14.docx</t>
+          <t>october 2024 dgvp ii class c.pdf</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -2100,15 +2100,15 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>trading</t>
+          <t>profile</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1095</v>
+        <v>838</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>optima global trading fund manager profiles 10_31_24.pptx</t>
+          <t>3.1.3 k-fit fund profile (july 2024) vf.pdf</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -2116,15 +2116,15 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>capital</t>
+          <t>journal</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>912</v>
+        <v>788</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>q2 2024 healthcare slides ra capital.pptx</t>
+          <t>journal.png</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -2132,15 +2132,15 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>storage</t>
+          <t>package</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>908</v>
+        <v>777</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>subdocs - prime storage fund ii cv llc ex.pdf</t>
+          <t>paradigm data package.xlsx</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -2199,7 +2199,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10346</v>
+        <v>9508</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -2215,7 +2215,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3261</v>
+        <v>2812</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -2231,11 +2231,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2814</v>
+        <v>2479</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>fft - fidelity bank statement 10.31.2024_8e7c8bd5-df9b-4bad-b1fd-98dfbc87f6d92024-11-04t15-28-48.pdf</t>
+          <t>2024-07-31 fidelity stmts - gayle averyt chrtb_acf09d6f-da22-4538-97f7-a6301bbcc2672024-09-30t16-47-33.pdf</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -2247,7 +2247,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2578</v>
+        <v>2422</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -2263,7 +2263,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2466</v>
+        <v>2243</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -2279,7 +2279,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2165</v>
+        <v>2010</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -2295,7 +2295,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1778</v>
+        <v>1646</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -2311,7 +2311,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1669</v>
+        <v>1411</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -2327,7 +2327,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1423</v>
+        <v>1303</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -2339,15 +2339,15 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>strategy</t>
+          <t>exposure</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1330</v>
+        <v>1179</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>gqm underlying strategy returns_september 2024.xlsx</t>
+          <t>gtf exposure snapshot - sep 2024.xlsx</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -2355,15 +2355,15 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>december</t>
+          <t>strategy</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1269</v>
+        <v>1165</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>atomiclabsiii_atomic labs iii l.p. - lp privacy notice (final - december 2022).pdf</t>
+          <t>gqm underlying strategy returns_september 2024.xlsx</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -2371,15 +2371,15 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>exposure</t>
+          <t>barclays</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1216</v>
+        <v>1066</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>gtf exposure snapshot - sep 2024.xlsx</t>
+          <t>ishares barclays aggregate bond fund prospectus 6_30_23.pdf</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -2387,15 +2387,15 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>barclays</t>
+          <t>snapshot</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1084</v>
+        <v>986</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>barclays hedge fund conference.docx</t>
+          <t>gtf exposure snapshot - sep 2024.xlsx</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -2403,15 +2403,15 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>november</t>
+          <t>designer</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1041</v>
+        <v>931</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>november 2024 msc notes.docx</t>
+          <t>interpolation.designer.cs</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -2419,15 +2419,15 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>snapshot</t>
+          <t>december</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1025</v>
+        <v>897</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>gtf exposure snapshot - sep 2024.xlsx</t>
+          <t>atomiclabsiii_atomic labs iii l.p. - lp privacy notice (final - december 2022).pdf</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -2482,15 +2482,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>statement</t>
+          <t>agreement</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4753</v>
+        <v>2728</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>fft - fidelity bank statement 10.31.2024_8e7c8bd5-df9b-4bad-b1fd-98dfbc87f6d92024-11-04t15-28-48.pdf</t>
+          <t>membership interest transfer agreement.pdf</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -2498,15 +2498,15 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>agreement</t>
+          <t>tradeaway</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3787</v>
+        <v>2391</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>membership interest transfer agreement.pdf</t>
+          <t>anet tradeaway 3 23 15 (ms).xls</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -2514,15 +2514,15 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>tradeaway</t>
+          <t>inventory</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2391</v>
+        <v>1510</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>anet tradeaway 3 23 15 (ms).xls</t>
+          <t>decommission &amp; moving items inventory list.xlsx</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -2534,7 +2534,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1657</v>
+        <v>1392</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -2546,15 +2546,15 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>inventory</t>
+          <t>insurance</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1580</v>
+        <v>1281</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>decommission &amp; moving items inventory list.xlsx</t>
+          <t>adler 2019 irrevocable insurance trust.pdf</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -2562,15 +2562,15 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>appraisal</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1432</v>
+        <v>1064</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>adler 2019 irrevocable insurance trust.pdf</t>
+          <t>john paul mordente - 1. internal appraisal - pb - 20240530_2acbe994-c3ff-41fc-9954-30f544d6a4102024-05-31t11-13-06.pdf</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -2578,15 +2578,15 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>appraisal</t>
+          <t>alphabeta</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1127</v>
+        <v>1039</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>john paul mordente - 1. internal appraisal - pb - 20240530_2acbe994-c3ff-41fc-9954-30f544d6a4102024-05-31t11-13-06.pdf</t>
+          <t>alphabeta summary (portrait) v1.pptx</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -2594,15 +2594,15 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>september</t>
+          <t>rebalance</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1102</v>
+        <v>888</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>september 2024</t>
+          <t>rebalance exchange amount.pdf</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -2610,15 +2610,15 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>alphabeta</t>
+          <t>september</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1044</v>
+        <v>829</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>alphabeta summary (portrait) v1.pptx</t>
+          <t>optima healthcare and biotech fund overview september 24.pptx</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -2626,15 +2626,15 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>rebalance</t>
+          <t>pomerantz</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>926</v>
+        <v>773</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>rebalance exchange amount.pdf</t>
+          <t>2024.09.30 jason sager pomerantz individual_4ab875fe-3464-422e-a553-9dd2f89492c62024-10-24t10-36-37.pdf</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -2646,7 +2646,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>833</v>
+        <v>771</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -2662,7 +2662,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>820</v>
+        <v>764</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -2674,15 +2674,15 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>pomerantz</t>
+          <t>documents</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>813</v>
+        <v>728</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2024.09.30 jason sager pomerantz individual_4ab875fe-3464-422e-a553-9dd2f89492c62024-10-24t10-36-37.pdf</t>
+          <t>colligo documents</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -2690,15 +2690,15 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>portfolio</t>
+          <t>revocable</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>782</v>
+        <v>709</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>haron marketables portfolio.png</t>
+          <t>2024.09.30 bertley sager revocable trust_a525fe09-6b29-462c-9d90-e2e9a128d63a2024-10-24t10-47-34.pdf</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -2706,15 +2706,15 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>documents</t>
+          <t>resources</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>773</v>
+        <v>696</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>colligo documents</t>
+          <t>2022.12.31 appian natural resources fund lp - fs signed.pdf</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -2773,7 +2773,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3053</v>
+        <v>2911</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -2789,7 +2789,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2316</v>
+        <v>2011</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -2805,7 +2805,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1044</v>
+        <v>1025</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2821,11 +2821,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>911</v>
+        <v>798</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>optima healthcare &amp; biotech manager profiles september 24.pptx</t>
+          <t>optima healthcare and biotech fund overview september 24.pptx</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -2833,15 +2833,15 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>financials</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>800</v>
+        <v>631</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>greenoaks iv 9.30.24 financials.pdf</t>
+          <t>bracco historical data 2024.08.xlsx</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -2849,15 +2849,15 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>individual</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>723</v>
+        <v>535</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>bracco historical data 2024.08.xlsx</t>
+          <t>ryan owens - individual application.pdf</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -2865,15 +2865,15 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>individual</t>
+          <t>securities</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>582</v>
+        <v>478</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ryan owens - individual application.pdf</t>
+          <t>thrive ix - fund formation securities law opinion (7.31.2024 closing).pdf</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -2881,15 +2881,15 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>supplement</t>
+          <t>properties</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>559</v>
+        <v>453</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>orent - ar ppm supplement number 1.pdf</t>
+          <t>star mountain iv - pileated properties - 2023 k-1_7f35bf10-8ad4-4eba-8710-f15f4ef295e42024-08-08t19-54-58.pdf</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -2897,15 +2897,15 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>statements</t>
+          <t>newsletter</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>531</v>
+        <v>410</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2022-07-23_financial statements.pdf</t>
+          <t>q3 2024 fund iii newsletter.pdf</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -2913,15 +2913,15 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>securities</t>
+          <t>screenshot</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>522</v>
+        <v>391</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>thrive ix - fund formation securities law opinion (7.31.2024 closing).pdf</t>
+          <t>screenshot 2023-10-18 at 4.05.13 pm.png</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -2929,15 +2929,15 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>agreements</t>
+          <t>charitable</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>518</v>
+        <v>380</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>llc agreements - h&amp;b llc &amp; gt llc_39b2cf96-b09e-46d5-95ad-5ad0ba8cd43d2024-10-22t15-58-06.zip</t>
+          <t>2024.09.30 elaine marieb charitable foundation pq_c3917d1a-d949-40db-8a63-a1ad73b680942024-10-23t15-35-40.pdf</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -2945,15 +2945,15 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>properties</t>
+          <t>agreements</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>470</v>
+        <v>378</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>star mountain iv - pileated properties - 2023 k-1_7f35bf10-8ad4-4eba-8710-f15f4ef295e42024-08-08t19-54-58.pdf</t>
+          <t>llc agreements - h&amp;b llc &amp; gt llc_39b2cf96-b09e-46d5-95ad-5ad0ba8cd43d2024-10-22t15-58-06.zip</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -2961,15 +2961,15 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>newsletter</t>
+          <t>strategies</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>412</v>
+        <v>363</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>q3 2024 fund iii newsletter.pdf</t>
+          <t>blackstone private equity strategies fund (bxpe)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -2977,15 +2977,15 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>screenshot</t>
+          <t>bloomfield</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>409</v>
+        <v>352</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>screenshot 2023-10-18 at 4.05.13 pm.png</t>
+          <t>bloomfield scott.pdf</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -2993,15 +2993,15 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>charitable</t>
+          <t>workpapers</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>408</v>
+        <v>315</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2024.09.30 elaine marieb charitable foundation pq_c3917d1a-d949-40db-8a63-a1ad73b680942024-10-23t15-35-40.pdf</t>
+          <t>recurring exp budget workpapers 2023_8cf0733a-a0be-4b8c-877e-e4b0fe2fa8ac2023-02-08t15-15-40.pdf</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -3056,15 +3056,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>investments</t>
+          <t>opportunity</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1848</v>
+        <v>1400</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>lerner - lel &amp; icl investments.pdf</t>
+          <t>jlp credit opportunity fund - september 2024.pdf</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -3072,15 +3072,15 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>opportunity</t>
+          <t>categorizer</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1474</v>
+        <v>863</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>jlp credit opportunity fund - september 2024.pdf</t>
+          <t>categorizer</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -3088,15 +3088,15 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>categorizer</t>
+          <t>application</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>872</v>
+        <v>744</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>categorizer</t>
+          <t>barker, elliott_immigration application receipt_form i-797c_732d9739-ac4d-4f8e-83f1-723e3b607ddf2024-09-12t09-47-37.pdf</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -3104,15 +3104,15 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>application</t>
+          <t>diversified</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>805</v>
+        <v>530</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>barker, elliott_immigration application receipt_form i-797c_732d9739-ac4d-4f8e-83f1-723e3b607ddf2024-09-12t09-47-37.pdf</t>
+          <t>2024 q2 diversified arbitrage fund - review book.pdf</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -3120,15 +3120,15 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>performance</t>
+          <t>spreadsheet</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>783</v>
+        <v>517</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>semi-liquid performance.xlsx</t>
+          <t>d-family credit exposure master spreadsheet.xlsx</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -3136,15 +3136,15 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>alternative</t>
+          <t>certificate</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>608</v>
+        <v>495</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>acl alternative fund - 31 december 2023 - final.pdf</t>
+          <t>orent - certificate of amendment.pdf</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -3152,15 +3152,15 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>certificate</t>
+          <t>renaissance</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>590</v>
+        <v>463</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>orent - certificate of amendment.pdf</t>
+          <t>thomas s. renaissance institutional equities fund llc - alpha analysis thru 4.30.2024.xlsx</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -3172,11 +3172,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>589</v>
+        <v>443</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>reports transaction completed - j.p. morgan access_fcc53d8f-e5eb-479b-9a13-b99b93a6b8262024-10-25t09-07-21.pdf</t>
+          <t>jackier transaction 1.png</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -3184,15 +3184,15 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>diversified</t>
+          <t>allocations</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>589</v>
+        <v>388</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2024 q2 diversified arbitrage fund - review book.pdf</t>
+          <t>client allocations - funds.xlsx</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -3200,15 +3200,15 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>spreadsheet</t>
+          <t>irrevocable</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>555</v>
+        <v>385</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>d-family credit exposure master spreadsheet.xlsx</t>
+          <t>2024.09.30 iponohea irrevocable trust - security performance_38498a76-5767-4179-b3fa-b6df156b76a32024-10-30t11-36-22.pdf</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -3216,15 +3216,15 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>renaissance</t>
+          <t>sheet_class</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>532</v>
+        <v>329</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>thomas s. renaissance institutional equities fund llc - alpha analysis thru 4.30.2024.xlsx</t>
+          <t>2020 10 01_am global core_fact sheet_class b.pdf</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -3232,15 +3232,15 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>allocations</t>
+          <t>alternative</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>403</v>
+        <v>329</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>client allocations - funds.xlsx</t>
+          <t>acl alternative fund - 31 december 2023 - final.pdf</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -3248,15 +3248,15 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>development</t>
+          <t>suitability</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>400</v>
+        <v>290</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>fft optima product development committee overview aug 2024.pdf</t>
+          <t>suitability</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -3264,15 +3264,15 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>irrevocable</t>
+          <t>correlation</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>395</v>
+        <v>287</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2024.09.30 iponohea irrevocable trust - security performance_38498a76-5767-4179-b3fa-b6df156b76a32024-10-30t11-36-22.pdf</t>
+          <t>fernside_caxton dynamis ranking &amp; correlation.xlsx</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -3280,15 +3280,15 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>sheet_class</t>
+          <t>fundfactors</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>381</v>
+        <v>285</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2020 10 01_am global core_fact sheet_class b.pdf</t>
+          <t>fundfactors.aspx.cs</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>

</xml_diff>